<commit_message>
EPBDS-9079 Support new date type - Instant
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/DatatypeDates.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/DatatypeDates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FCE85C-5B9C-476A-B0E5-90BD0A2C05C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57922E4C-B041-4360-93A9-C57B1CACC7B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -161,6 +161,21 @@
   </si>
   <si>
     <t>2019-10-10T10:15:00Z[UTC]</t>
+  </si>
+  <si>
+    <t>Instant</t>
+  </si>
+  <si>
+    <t>instantDate2</t>
+  </si>
+  <si>
+    <t>java.time.Instant</t>
+  </si>
+  <si>
+    <t>2019-10-10T17:15:00Z</t>
+  </si>
+  <si>
+    <t>instantDate</t>
   </si>
 </sst>
 </file>
@@ -265,11 +280,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -626,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:J18"/>
+  <dimension ref="B3:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,30 +663,30 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="F7" s="11" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="F7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -911,6 +928,50 @@
       </c>
       <c r="H18" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="11" t="str">
+        <f t="shared" ref="F19" si="16">"_res_." &amp; C19</f>
+        <v>_res_.instantDate</v>
+      </c>
+      <c r="G19" s="11" t="str">
+        <f t="shared" ref="G19" si="17">C19</f>
+        <v>instantDate</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="12" t="str">
+        <f t="shared" ref="F20" si="18">"_res_." &amp; C20</f>
+        <v>_res_.instantDate2</v>
+      </c>
+      <c r="G20" s="12" t="str">
+        <f t="shared" ref="G20" si="19">C20</f>
+        <v>instantDate2</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -927,10 +988,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:D7"/>
+  <dimension ref="B3:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,50 +1001,60 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="C4:D4"/>

</xml_diff>